<commit_message>
finished results section. Only thing to do is Ecological Relevance and Conclusions
</commit_message>
<xml_diff>
--- a/python/models/Regressors/results/characteristic_length/characteristic_length.xlsx
+++ b/python/models/Regressors/results/characteristic_length/characteristic_length.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkerkingfournier/Desktop/characteristic_length/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkerkingfournier/Documents/Development/workspace/projects/Ecological-Inference/python/models/Regressors/results/characteristic_length/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -362,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1436,6 +1436,26 @@
         <v>0.27342063188552801</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <f>MIN(B2:B41)</f>
+        <v>0.26033341884612998</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:D43" si="0">MIN(C2:C41)</f>
+        <v>0.11141914129257199</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>5.5744864046573597E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <f>AVERAGE(B43:D43)</f>
+        <v>0.14249914139509184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>